<commit_message>
test two brackets from same name
</commit_message>
<xml_diff>
--- a/brackets/bracket_2022_CameronTest1.xlsx
+++ b/brackets/bracket_2022_CameronTest1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caharris\hockey\pools\playoffs_2022\nhl_playoff_challenge2022\brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B08C08B-0394-4023-9BEC-C41280A3B988}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F430CD-82E3-407E-B3E1-C5E8AAA1D835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,16 +226,16 @@
     <t>Your Name:</t>
   </si>
   <si>
+    <t>Pasternak</t>
+  </si>
+  <si>
+    <t>tie_breaker</t>
+  </si>
+  <si>
+    <t>entrant_name</t>
+  </si>
+  <si>
     <t>Cameron Harris</t>
-  </si>
-  <si>
-    <t>Pasternak</t>
-  </si>
-  <si>
-    <t>tie_breaker</t>
-  </si>
-  <si>
-    <t>entrant_name</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1633,7 @@
       <c r="C12" s="28"/>
       <c r="D12" s="48"/>
       <c r="E12" s="78" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="79"/>
       <c r="G12" s="50"/>
@@ -1672,7 +1672,7 @@
         <v>51</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G14" s="64"/>
       <c r="H14" s="26" t="s">
@@ -1934,10 +1934,10 @@
         <v>49</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>